<commit_message>
Dil Desteği + Model İlişki Düzenleme
Dil Desteği + Model İlişki Düzenleme
</commit_message>
<xml_diff>
--- a/Şema.xlsx
+++ b/Şema.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13860" windowHeight="6135" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13860" windowHeight="6135" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="License" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="85">
   <si>
     <t>id</t>
   </si>
@@ -141,9 +141,6 @@
     <t>Soyad</t>
   </si>
   <si>
-    <t>Lakap</t>
-  </si>
-  <si>
     <t>Kullanıcı Adı</t>
   </si>
   <si>
@@ -187,9 +184,6 @@
   </si>
   <si>
     <t>Lastname</t>
-  </si>
-  <si>
-    <t>Nickname</t>
   </si>
   <si>
     <t>Username</t>
@@ -522,6 +516,12 @@
   </si>
   <si>
     <t>Language</t>
+  </si>
+  <si>
+    <t>NOT NULL</t>
+  </si>
+  <si>
+    <t>true</t>
   </si>
 </sst>
 </file>
@@ -702,10 +702,10 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1004,7 +1004,7 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>4</v>
@@ -1021,23 +1021,23 @@
         <v>14</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>5</v>
@@ -1048,10 +1048,10 @@
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="19" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>28</v>
@@ -1059,10 +1059,10 @@
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="19" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>29</v>
@@ -1076,7 +1076,7 @@
         <v>23</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1100,7 +1100,7 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>5</v>
@@ -1117,29 +1117,29 @@
         <v>14</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
@@ -1150,7 +1150,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1162,8 +1162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AB36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1186,7 +1186,7 @@
   <sheetData>
     <row r="2" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>1</v>
@@ -1207,33 +1207,39 @@
         <v>14</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E3" s="21"/>
     </row>
     <row r="4" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E4" s="21"/>
+      <c r="F4" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="5" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E5" s="21"/>
+      <c r="F5" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="6" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
@@ -1243,10 +1249,10 @@
         <v>10</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="E6" s="22" t="s">
-        <v>72</v>
+        <v>60</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>70</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="10"/>
@@ -1254,7 +1260,7 @@
     </row>
     <row r="7" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>11</v>
@@ -1262,12 +1268,12 @@
       <c r="D7" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="22"/>
+      <c r="E7" s="23"/>
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>3</v>
@@ -1275,12 +1281,12 @@
       <c r="D8" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="23"/>
+      <c r="E8" s="22"/>
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>4</v>
@@ -1288,61 +1294,73 @@
       <c r="D9" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="23"/>
+      <c r="E9" s="22"/>
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E10" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="E10" s="24" t="s">
-        <v>81</v>
+      <c r="F10" t="s">
+        <v>83</v>
       </c>
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E11" s="24"/>
+      <c r="F11" t="s">
+        <v>83</v>
+      </c>
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E12" s="24"/>
+      <c r="F12" t="s">
+        <v>83</v>
+      </c>
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E13" s="24"/>
+      <c r="F13" t="s">
+        <v>83</v>
+      </c>
       <c r="U13" s="1"/>
       <c r="V13" s="1"/>
       <c r="W13" s="1"/>
@@ -1354,16 +1372,18 @@
     </row>
     <row r="14" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D14" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" s="21"/>
+      <c r="F14" t="s">
         <v>83</v>
       </c>
-      <c r="E14" s="21"/>
-      <c r="F14" s="2"/>
       <c r="G14" s="10"/>
       <c r="U14" s="1"/>
       <c r="V14" s="1"/>
@@ -1379,12 +1399,15 @@
         <v>21</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E15" s="21"/>
+      <c r="F15" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="16" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E16" s="4"/>
@@ -1436,20 +1459,20 @@
   <dimension ref="B1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:D13"/>
+      <selection activeCell="B15" sqref="B15:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>3</v>
@@ -1466,7 +1489,7 @@
         <v>14</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1482,10 +1505,10 @@
     </row>
     <row r="5" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>34</v>
@@ -1493,10 +1516,10 @@
     </row>
     <row r="6" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>35</v>
@@ -1504,32 +1527,32 @@
     </row>
     <row r="7" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>53</v>
+      <c r="B8" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>52</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>54</v>
+      <c r="B9" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>38</v>
@@ -1537,10 +1560,10 @@
     </row>
     <row r="10" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>39</v>
@@ -1548,10 +1571,10 @@
     </row>
     <row r="11" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>40</v>
@@ -1559,10 +1582,10 @@
     </row>
     <row r="12" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="17" t="s">
-        <v>79</v>
+        <v>21</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>41</v>
@@ -1570,10 +1593,10 @@
     </row>
     <row r="13" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="17" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>42</v>
@@ -1581,26 +1604,16 @@
     </row>
     <row r="14" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
+    <row r="15" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1619,7 +1632,7 @@
   <dimension ref="B2:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1631,7 +1644,7 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>7</v>
@@ -1648,18 +1661,18 @@
         <v>14</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
@@ -1670,7 +1683,7 @@
         <v>17</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1682,8 +1695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1695,7 +1708,7 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>6</v>
@@ -1712,29 +1725,29 @@
         <v>14</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
@@ -1745,23 +1758,23 @@
         <v>17</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>3</v>
@@ -1792,7 +1805,7 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>2</v>
@@ -1809,12 +1822,12 @@
         <v>14</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>24</v>
@@ -1825,7 +1838,7 @@
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>15</v>
@@ -1856,7 +1869,7 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>9</v>
@@ -1873,29 +1886,29 @@
         <v>14</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
@@ -1906,7 +1919,7 @@
         <v>17</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
@@ -1914,15 +1927,15 @@
         <v>23</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>3</v>

</xml_diff>